<commit_message>
feat: notebook to python files
</commit_message>
<xml_diff>
--- a/results/disgenet_elbow.xlsx
+++ b/results/disgenet_elbow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\gene-disease-gnn\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DE1A542-5861-40EA-AE1F-CB870C628704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8739538-2056-47D4-9D46-E3E78329571F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{E457D8DB-CE38-4117-9557-F54BBE2E3521}"/>
   </bookViews>
@@ -33,6 +33,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>gene-disease association</t>
+  </si>
+  <si>
+    <t>number of diseases that has that much association</t>
+  </si>
+  <si>
+    <t>the remaining number of gene-disease association if we cut here the dataset</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67,8 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -120,10 +137,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Disease number</a:t>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Diseases'</a:t>
             </a:r>
-            <a:endParaRPr lang="hu-HU"/>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> gene</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> number</a:t>
+            </a:r>
+            <a:endParaRPr lang="hu-HU" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -189,618 +214,618 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Munka1!$A$1:$A$100</c:f>
+              <c:f>Munka1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$C$1:$C$100</c:f>
+              <c:f>Munka1!$C$2:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>569</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>585</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>629</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>802</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>837</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>868</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>897</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>939</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>979</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1043</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1109</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1246</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1356</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1449</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1559</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1655</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1814</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2240</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2587</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3642</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5086</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>10967</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5086</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3642</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2587</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2240</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1814</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1655</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1559</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1449</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1356</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1246</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1180</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1109</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1043</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>979</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>939</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>897</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>868</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>837</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>802</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>776</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>758</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>744</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>710</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>674</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>639</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>629</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>615</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>585</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>569</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>556</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>530</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>520</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>491</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>479</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>466</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>455</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>442</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>436</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>429</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>424</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>413</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>411</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>394</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>385</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>370</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>346</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>343</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>337</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>326</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>311</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>309</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>307</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>304</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>299</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>297</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>297</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>292</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>272</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>269</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>255</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>251</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>249</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>249</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>242</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>235</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>218</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>214</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>207</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>203</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,6 +852,7 @@
         <c:axId val="952894959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -844,6 +870,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Diseases'</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> gene number</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -906,6 +992,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Diseases number</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1026,10 +1168,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1"/>
               <a:t>Remaining gene-disease connections</a:t>
             </a:r>
-            <a:endParaRPr lang="hu-HU"/>
+            <a:endParaRPr lang="hu-HU" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1095,618 +1237,618 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Munka1!$A$1:$A$100</c:f>
+              <c:f>Munka1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$B$1:$B$100</c:f>
+              <c:f>Munka1!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
+                  <c:v>37390</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37587</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38165</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38355</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38355</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38541</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38541</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38814</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39171</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39345</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39947</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40117</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40369</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40618</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40782</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41187</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41427</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41743</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41743</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41897</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42726</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43244</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43463</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43535</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43677</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44842</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45177</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45177</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45307</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45435</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>45624</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>45810</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45932</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>46052</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46465</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>46929</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>47556</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>47892</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>48057</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>48381</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48805</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49065</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49320</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50070</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50511</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>50847</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>51317</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>51409</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>51904</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>52124</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>52425</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>52677</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>52923</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>53203</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>53632</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>54126</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>54570</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>54894</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>55594</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>55934</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>56792</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>57208</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>57704</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>58604</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>59010</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>59290</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>60235</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>61171</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>62021</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>62357</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>62771</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>63343</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>64078</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>64698</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>65249</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>66005</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>66685</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>67709</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>68699</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>69693</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>70551</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>71871</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>72894</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>73994</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>74858</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>76130</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>77481</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>78879</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>80614</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>82258</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>84190</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>87078</c:v>
+                </c:pt>
+                <c:pt idx="99">
                   <c:v>92959</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>87078</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>84190</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>82258</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>80614</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>78879</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>77481</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>76130</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>74858</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>73994</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>72894</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>71871</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>70551</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>69693</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>68699</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>67709</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>66685</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>66005</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>65249</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>64698</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>64078</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>63343</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>62771</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>62357</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>62021</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>61171</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>60235</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>59290</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>59010</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>58604</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>57704</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>57208</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>56792</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>55934</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>55594</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>54894</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>54570</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>54126</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>53632</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>53203</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>52923</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>52677</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>52425</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>52124</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>51904</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>51409</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>51317</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>50847</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>50511</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50070</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>49320</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>49065</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>48805</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>48381</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>48057</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>47892</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>47556</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>46929</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>46465</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>46052</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>45932</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>45810</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>45624</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>45435</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>45307</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>45177</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>45177</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>44842</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>44026</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>43957</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>43677</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>43535</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>43463</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>43244</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>42726</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>42201</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>41897</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>41743</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>41743</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>41427</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>41187</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>40782</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>40618</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>40369</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>40117</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>39947</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>39345</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>39171</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>39083</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>38994</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>38814</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>38541</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>38541</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>38355</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>38355</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>38165</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>37781</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>37587</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>37489</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>37390</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,6 +1875,7 @@
         <c:axId val="1161279071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1750,6 +1893,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Diseases' gene number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1812,6 +2017,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Gene-disease</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> number</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3015,15 +3280,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3050,16 +3315,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3404,562 +3669,567 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F88AB79-5890-492F-AAA0-2786A84C87B7}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B1:B100"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>92959</v>
-      </c>
-      <c r="C1">
-        <v>10967</v>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="B2">
-        <v>87078</v>
+        <v>37390</v>
       </c>
       <c r="C2">
-        <v>5086</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="B3">
-        <v>84190</v>
+        <v>37489</v>
       </c>
       <c r="C3">
-        <v>3642</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B4">
-        <v>82258</v>
+        <v>37587</v>
       </c>
       <c r="C4">
-        <v>2998</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="B5">
-        <v>80614</v>
+        <v>37781</v>
       </c>
       <c r="C5">
-        <v>2587</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="B6">
-        <v>78879</v>
+        <v>38165</v>
       </c>
       <c r="C6">
-        <v>2240</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="B7">
-        <v>77481</v>
+        <v>38355</v>
       </c>
       <c r="C7">
-        <v>2007</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="B8">
-        <v>76130</v>
+        <v>38355</v>
       </c>
       <c r="C8">
-        <v>1814</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="B9">
-        <v>74858</v>
+        <v>38541</v>
       </c>
       <c r="C9">
-        <v>1655</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="B10">
-        <v>73994</v>
+        <v>38541</v>
       </c>
       <c r="C10">
-        <v>1559</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="B11">
-        <v>72894</v>
+        <v>38814</v>
       </c>
       <c r="C11">
-        <v>1449</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="B12">
-        <v>71871</v>
+        <v>38994</v>
       </c>
       <c r="C12">
-        <v>1356</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="B13">
-        <v>70551</v>
+        <v>39083</v>
       </c>
       <c r="C13">
-        <v>1246</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B14">
-        <v>69693</v>
+        <v>39171</v>
       </c>
       <c r="C14">
-        <v>1180</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="B15">
-        <v>68699</v>
+        <v>39345</v>
       </c>
       <c r="C15">
-        <v>1109</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="B16">
-        <v>67709</v>
+        <v>39947</v>
       </c>
       <c r="C16">
-        <v>1043</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="B17">
-        <v>66685</v>
+        <v>40117</v>
       </c>
       <c r="C17">
-        <v>979</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B18">
-        <v>66005</v>
+        <v>40369</v>
       </c>
       <c r="C18">
-        <v>939</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B19">
-        <v>65249</v>
+        <v>40618</v>
       </c>
       <c r="C19">
-        <v>897</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B20">
-        <v>64698</v>
+        <v>40782</v>
       </c>
       <c r="C20">
-        <v>868</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B21">
-        <v>64078</v>
+        <v>41187</v>
       </c>
       <c r="C21">
-        <v>837</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="B22">
-        <v>63343</v>
+        <v>41427</v>
       </c>
       <c r="C22">
-        <v>802</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="B23">
-        <v>62771</v>
+        <v>41743</v>
       </c>
       <c r="C23">
-        <v>776</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="B24">
-        <v>62357</v>
+        <v>41743</v>
       </c>
       <c r="C24">
-        <v>758</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B25">
-        <v>62021</v>
+        <v>41897</v>
       </c>
       <c r="C25">
-        <v>744</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B26">
-        <v>61171</v>
+        <v>42201</v>
       </c>
       <c r="C26">
-        <v>710</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B27">
-        <v>60235</v>
+        <v>42726</v>
       </c>
       <c r="C27">
-        <v>674</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="B28">
-        <v>59290</v>
+        <v>43244</v>
       </c>
       <c r="C28">
-        <v>639</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B29">
-        <v>59010</v>
+        <v>43463</v>
       </c>
       <c r="C29">
-        <v>629</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B30">
-        <v>58604</v>
+        <v>43535</v>
       </c>
       <c r="C30">
-        <v>615</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B31">
-        <v>57704</v>
+        <v>43677</v>
       </c>
       <c r="C31">
-        <v>585</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B32">
-        <v>57208</v>
+        <v>43957</v>
       </c>
       <c r="C32">
-        <v>569</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B33">
-        <v>56792</v>
+        <v>44026</v>
       </c>
       <c r="C33">
-        <v>556</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B34">
-        <v>55934</v>
+        <v>44842</v>
       </c>
       <c r="C34">
-        <v>530</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B35">
-        <v>55594</v>
+        <v>45177</v>
       </c>
       <c r="C35">
-        <v>520</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B36">
-        <v>54894</v>
+        <v>45177</v>
       </c>
       <c r="C36">
-        <v>500</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B37">
-        <v>54570</v>
+        <v>45307</v>
       </c>
       <c r="C37">
-        <v>491</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B38">
-        <v>54126</v>
+        <v>45435</v>
       </c>
       <c r="C38">
-        <v>479</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B39">
-        <v>53632</v>
+        <v>45624</v>
       </c>
       <c r="C39">
-        <v>466</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B40">
-        <v>53203</v>
+        <v>45810</v>
       </c>
       <c r="C40">
-        <v>455</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B41">
-        <v>52923</v>
+        <v>45932</v>
       </c>
       <c r="C41">
-        <v>448</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B42">
-        <v>52677</v>
+        <v>46052</v>
       </c>
       <c r="C42">
-        <v>442</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B43">
-        <v>52425</v>
+        <v>46465</v>
       </c>
       <c r="C43">
-        <v>436</v>
+        <v>318</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B44">
-        <v>52124</v>
+        <v>46929</v>
       </c>
       <c r="C44">
-        <v>429</v>
+        <v>326</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B45">
-        <v>51904</v>
+        <v>47556</v>
       </c>
       <c r="C45">
-        <v>424</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B46">
-        <v>51409</v>
+        <v>47892</v>
       </c>
       <c r="C46">
-        <v>413</v>
+        <v>343</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B47">
-        <v>51317</v>
+        <v>48057</v>
       </c>
       <c r="C47">
-        <v>411</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B48">
-        <v>50847</v>
+        <v>48381</v>
       </c>
       <c r="C48">
-        <v>401</v>
+        <v>352</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B49">
-        <v>50511</v>
+        <v>48805</v>
       </c>
       <c r="C49">
-        <v>394</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50">
-        <v>50070</v>
+        <v>49065</v>
       </c>
       <c r="C50">
-        <v>385</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3975,544 +4245,558 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>49065</v>
+        <v>50070</v>
       </c>
       <c r="C52">
-        <v>365</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B53">
-        <v>48805</v>
+        <v>50511</v>
       </c>
       <c r="C53">
-        <v>360</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B54">
-        <v>48381</v>
+        <v>50847</v>
       </c>
       <c r="C54">
-        <v>352</v>
+        <v>401</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B55">
-        <v>48057</v>
+        <v>51317</v>
       </c>
       <c r="C55">
-        <v>346</v>
+        <v>411</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B56">
-        <v>47892</v>
+        <v>51409</v>
       </c>
       <c r="C56">
-        <v>343</v>
+        <v>413</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B57">
-        <v>47556</v>
+        <v>51904</v>
       </c>
       <c r="C57">
-        <v>337</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B58">
-        <v>46929</v>
+        <v>52124</v>
       </c>
       <c r="C58">
-        <v>326</v>
+        <v>429</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B59">
-        <v>46465</v>
+        <v>52425</v>
       </c>
       <c r="C59">
-        <v>318</v>
+        <v>436</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B60">
-        <v>46052</v>
+        <v>52677</v>
       </c>
       <c r="C60">
-        <v>311</v>
+        <v>442</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B61">
-        <v>45932</v>
+        <v>52923</v>
       </c>
       <c r="C61">
-        <v>309</v>
+        <v>448</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B62">
-        <v>45810</v>
+        <v>53203</v>
       </c>
       <c r="C62">
-        <v>307</v>
+        <v>455</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B63">
-        <v>45624</v>
+        <v>53632</v>
       </c>
       <c r="C63">
-        <v>304</v>
+        <v>466</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B64">
-        <v>45435</v>
+        <v>54126</v>
       </c>
       <c r="C64">
-        <v>301</v>
+        <v>479</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B65">
-        <v>45307</v>
+        <v>54570</v>
       </c>
       <c r="C65">
-        <v>299</v>
+        <v>491</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="B66">
-        <v>45177</v>
+        <v>54894</v>
       </c>
       <c r="C66">
-        <v>297</v>
+        <v>500</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B67">
-        <v>45177</v>
+        <v>55594</v>
       </c>
       <c r="C67">
-        <v>297</v>
+        <v>520</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B68">
-        <v>44842</v>
+        <v>55934</v>
       </c>
       <c r="C68">
-        <v>292</v>
+        <v>530</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B69">
-        <v>44026</v>
+        <v>56792</v>
       </c>
       <c r="C69">
-        <v>280</v>
+        <v>556</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B70">
-        <v>43957</v>
+        <v>57208</v>
       </c>
       <c r="C70">
-        <v>279</v>
+        <v>569</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B71">
-        <v>43677</v>
+        <v>57704</v>
       </c>
       <c r="C71">
-        <v>275</v>
+        <v>585</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="B72">
-        <v>43535</v>
+        <v>58604</v>
       </c>
       <c r="C72">
-        <v>273</v>
+        <v>615</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B73">
-        <v>43463</v>
+        <v>59010</v>
       </c>
       <c r="C73">
-        <v>272</v>
+        <v>629</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="B74">
-        <v>43244</v>
+        <v>59290</v>
       </c>
       <c r="C74">
-        <v>269</v>
+        <v>639</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B75">
-        <v>42726</v>
+        <v>60235</v>
       </c>
       <c r="C75">
-        <v>262</v>
+        <v>674</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="B76">
-        <v>42201</v>
+        <v>61171</v>
       </c>
       <c r="C76">
-        <v>255</v>
+        <v>710</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B77">
-        <v>41897</v>
+        <v>62021</v>
       </c>
       <c r="C77">
-        <v>251</v>
+        <v>744</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="B78">
-        <v>41743</v>
+        <v>62357</v>
       </c>
       <c r="C78">
-        <v>249</v>
+        <v>758</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="B79">
-        <v>41743</v>
+        <v>62771</v>
       </c>
       <c r="C79">
-        <v>249</v>
+        <v>776</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="B80">
-        <v>41427</v>
+        <v>63343</v>
       </c>
       <c r="C80">
-        <v>245</v>
+        <v>802</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B81">
-        <v>41187</v>
+        <v>64078</v>
       </c>
       <c r="C81">
-        <v>242</v>
+        <v>837</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B82">
-        <v>40782</v>
+        <v>64698</v>
       </c>
       <c r="C82">
-        <v>237</v>
+        <v>868</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B83">
-        <v>40618</v>
+        <v>65249</v>
       </c>
       <c r="C83">
-        <v>235</v>
+        <v>897</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="B84">
-        <v>40369</v>
+        <v>66005</v>
       </c>
       <c r="C84">
-        <v>232</v>
+        <v>939</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="B85">
-        <v>40117</v>
+        <v>66685</v>
       </c>
       <c r="C85">
-        <v>229</v>
+        <v>979</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="B86">
-        <v>39947</v>
+        <v>67709</v>
       </c>
       <c r="C86">
-        <v>227</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="B87">
-        <v>39345</v>
+        <v>68699</v>
       </c>
       <c r="C87">
-        <v>220</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="B88">
-        <v>39171</v>
+        <v>69693</v>
       </c>
       <c r="C88">
-        <v>218</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="B89">
-        <v>39083</v>
+        <v>70551</v>
       </c>
       <c r="C89">
-        <v>217</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="B90">
-        <v>38994</v>
+        <v>71871</v>
       </c>
       <c r="C90">
-        <v>216</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="B91">
-        <v>38814</v>
+        <v>72894</v>
       </c>
       <c r="C91">
-        <v>214</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="B92">
-        <v>38541</v>
+        <v>73994</v>
       </c>
       <c r="C92">
-        <v>211</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="B93">
-        <v>38541</v>
+        <v>74858</v>
       </c>
       <c r="C93">
-        <v>211</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="B94">
-        <v>38355</v>
+        <v>76130</v>
       </c>
       <c r="C94">
-        <v>209</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="B95">
-        <v>38355</v>
+        <v>77481</v>
       </c>
       <c r="C95">
-        <v>209</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="B96">
-        <v>38165</v>
+        <v>78879</v>
       </c>
       <c r="C96">
-        <v>207</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="B97">
-        <v>37781</v>
+        <v>80614</v>
       </c>
       <c r="C97">
-        <v>203</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="B98">
-        <v>37587</v>
+        <v>82258</v>
       </c>
       <c r="C98">
-        <v>201</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="B99">
-        <v>37489</v>
+        <v>84190</v>
       </c>
       <c r="C99">
-        <v>200</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="B100">
-        <v>37390</v>
+        <v>87078</v>
       </c>
       <c r="C100">
-        <v>199</v>
+        <v>5086</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>92959</v>
+      </c>
+      <c r="C101">
+        <v>10967</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C101">
+    <sortCondition descending="1" ref="A2:A101"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>